<commit_message>
Single Question added with image
</commit_message>
<xml_diff>
--- a/public/file/sample_questions.xlsx
+++ b/public/file/sample_questions.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="13">
   <si>
     <t>Question</t>
   </si>
@@ -47,6 +47,12 @@
   </si>
   <si>
     <t>Option4</t>
+  </si>
+  <si>
+    <t>Image</t>
+  </si>
+  <si>
+    <t>img.png</t>
   </si>
 </sst>
 </file>
@@ -385,62 +391,184 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75">
+    <row r="1" spans="1:8" ht="15.75">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="1"/>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
-        <v>2</v>
-      </c>
       <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>